<commit_message>
Common: Added maximum power for a mod
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/mods.xlsx
+++ b/upgrade/fixtures/mods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E41A934-A5A4-48C6-BACD-33550904A962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22781436-F70A-483E-A31B-28D11D2CEAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="4020" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2670" yWindow="5595" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>tab</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Dani Box 21700 MOD</t>
+  </si>
+  <si>
+    <t>power</t>
   </si>
 </sst>
 </file>
@@ -447,64 +450,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0888C51-D22A-4EB9-B572-2B7661763B22}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>